<commit_message>
asset : update fix
</commit_message>
<xml_diff>
--- a/storage/template/ASSET_LISTS.xlsx
+++ b/storage/template/ASSET_LISTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\iids\storage\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8FBE5F-2FE9-4D52-8D9F-37E486D4EC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A6B08B-C910-4AFD-BB13-DF2C1C5AF7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A6CA3622-90F2-4BB9-8AF2-2E15C4A379E8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>status</t>
   </si>
@@ -81,9 +81,6 @@
     <t>remark</t>
   </si>
   <si>
-    <t>storage</t>
-  </si>
-  <si>
     <t>package</t>
   </si>
   <si>
@@ -178,6 +175,15 @@
   </si>
   <si>
     <t>2021-08-20</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>acquisition</t>
   </si>
 </sst>
 </file>
@@ -607,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171F437A-DBD3-4EB5-B9D4-EC7D62D3AA77}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,17 +631,17 @@
     <col min="9" max="10" width="19.54296875" customWidth="1"/>
     <col min="11" max="11" width="18.6328125" customWidth="1"/>
     <col min="12" max="12" width="19.26953125" customWidth="1"/>
-    <col min="13" max="13" width="17.90625" customWidth="1"/>
-    <col min="14" max="14" width="17.26953125" style="4" customWidth="1"/>
-    <col min="15" max="17" width="12.36328125" customWidth="1"/>
-    <col min="18" max="19" width="20.6328125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="27.54296875" style="4" customWidth="1"/>
-    <col min="21" max="21" width="18.54296875" customWidth="1"/>
-    <col min="22" max="22" width="18" style="1" customWidth="1"/>
-    <col min="23" max="23" width="26.26953125" customWidth="1"/>
+    <col min="13" max="14" width="17.90625" customWidth="1"/>
+    <col min="15" max="15" width="17.26953125" style="4" customWidth="1"/>
+    <col min="16" max="18" width="12.36328125" customWidth="1"/>
+    <col min="19" max="20" width="20.6328125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="27.54296875" style="4" customWidth="1"/>
+    <col min="22" max="22" width="18.54296875" customWidth="1"/>
+    <col min="23" max="23" width="18" style="1" customWidth="1"/>
+    <col min="24" max="24" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -675,143 +681,152 @@
       <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1"/>
+      <c r="W1"/>
+    </row>
+    <row r="2" spans="1:23" s="9" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T1"/>
-      <c r="V1"/>
-    </row>
-    <row r="2" spans="1:22" s="9" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="12">
         <v>1300</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="O2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="T2" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="9" customFormat="1" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" s="9" customFormat="1" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="12">
         <v>4000</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="O3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="Q3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asset & Rental : implement space
</commit_message>
<xml_diff>
--- a/storage/template/ASSET_LISTS.xlsx
+++ b/storage/template/ASSET_LISTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\iids\storage\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656869FA-6CD5-43AA-9639-B091AEC424E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D948C56-1CCF-4180-9171-DE846E65F812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A6CA3622-90F2-4BB9-8AF2-2E15C4A379E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A6CA3622-90F2-4BB9-8AF2-2E15C4A379E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>status</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>RABBIT IT</t>
-  </si>
-  <si>
-    <t>office</t>
   </si>
   <si>
     <t>1</t>
@@ -622,7 +619,7 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -661,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
@@ -691,10 +688,10 @@
         <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>14</v>
@@ -703,13 +700,13 @@
         <v>0</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V1"/>
       <c r="X1"/>
@@ -728,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>23</v>
@@ -740,7 +737,7 @@
         <v>28</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>35</v>
@@ -758,7 +755,7 @@
         <v>32</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>37</v>
@@ -767,16 +764,16 @@
         <v>14</v>
       </c>
       <c r="R2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="U2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="9" customFormat="1" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -793,7 +790,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>24</v>
@@ -805,7 +802,7 @@
         <v>29</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>36</v>
@@ -823,25 +820,25 @@
         <v>33</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>